<commit_message>
finish notes for 2021-12-02
</commit_message>
<xml_diff>
--- a/academic/Eaton_et_al._2021_Plagued_by_a_cryptic_clock.xlsx
+++ b/academic/Eaton_et_al._2021_Plagued_by_a_cryptic_clock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\obsidian-public\academic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCC01C8-31FF-4AE9-A279-2B74523EEBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616FDF71-C15D-432E-A7FD-2BD9EFD2BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table SI 1" sheetId="1" r:id="rId1"/>
@@ -2048,6 +2048,7 @@
     <xf numFmtId="0" fontId="22" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2087,7 +2088,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2468,17 +2468,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -2929,16 +2929,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="118" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="119"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="120"/>
     </row>
     <row r="2" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -3314,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3336,15 +3336,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="116" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
       <c r="H1" s="56"/>
       <c r="I1" s="56"/>
       <c r="J1" s="56"/>
@@ -3875,65 +3875,65 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G16" s="10"/>
-      <c r="K16" s="128"/>
+      <c r="K16" s="115"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.35">
       <c r="G17" s="10"/>
-      <c r="K17" s="128"/>
+      <c r="K17" s="115"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.35">
       <c r="G18" s="10"/>
-      <c r="K18" s="128"/>
+      <c r="K18" s="115"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="K19" s="128"/>
+      <c r="K19" s="115"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="K20" s="128"/>
+      <c r="K20" s="115"/>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="K21" s="128"/>
+      <c r="K21" s="115"/>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="K22" s="128"/>
+      <c r="K22" s="115"/>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="K23" s="128"/>
+      <c r="K23" s="115"/>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="K24" s="128"/>
+      <c r="K24" s="115"/>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="K25" s="128"/>
+      <c r="K25" s="115"/>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="K26" s="128"/>
+      <c r="K26" s="115"/>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="K27" s="128"/>
+      <c r="K27" s="115"/>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="K28" s="128"/>
+      <c r="K28" s="115"/>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D29" s="10"/>
@@ -3956,8 +3956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3978,48 +3978,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="124" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="124"/>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="125"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
+      <c r="N1" s="125"/>
+      <c r="O1" s="125"/>
+      <c r="P1" s="126"/>
     </row>
     <row r="2" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="121" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="120" t="s">
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="121" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="120" t="s">
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="121" t="s">
         <v>119</v>
       </c>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="122"/>
+      <c r="P2" s="123"/>
     </row>
     <row r="3" spans="1:23" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="57" t="s">
@@ -4856,13 +4856,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="124" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -4873,12 +4873,12 @@
     </row>
     <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="121" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="123"/>
       <c r="J2" s="93"/>
       <c r="K2" s="93"/>
       <c r="L2" s="93"/>
@@ -5169,46 +5169,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="127"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
     </row>
     <row r="2" spans="1:15" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="121" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="120" t="s">
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="123"/>
+      <c r="H2" s="121" t="s">
         <v>153</v>
       </c>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="120" t="s">
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="123"/>
+      <c r="L2" s="121" t="s">
         <v>155</v>
       </c>
-      <c r="M2" s="121"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="122"/>
+      <c r="O2" s="123"/>
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
@@ -5864,44 +5864,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
     </row>
     <row r="2" spans="1:14" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="121" t="s">
         <v>151</v>
       </c>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="120" t="s">
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="123"/>
+      <c r="G2" s="121" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="120" t="s">
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
+      <c r="K2" s="121" t="s">
         <v>155</v>
       </c>
-      <c r="L2" s="121"/>
-      <c r="M2" s="121"/>
-      <c r="N2" s="122"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="123"/>
     </row>
     <row r="3" spans="1:14" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="98" t="s">

</xml_diff>

<commit_message>
finish notes for 2021-12-06
</commit_message>
<xml_diff>
--- a/academic/Eaton_et_al._2021_Plagued_by_a_cryptic_clock.xlsx
+++ b/academic/Eaton_et_al._2021_Plagued_by_a_cryptic_clock.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktmea\Projects\obsidian-public\academic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616FDF71-C15D-432E-A7FD-2BD9EFD2BB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E340175D-8911-43CF-850B-4196E1F62AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table SI 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Table SI 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table SI 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Table SI 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Table SI 5" sheetId="5" r:id="rId5"/>
-    <sheet name="Table SI 6" sheetId="6" r:id="rId6"/>
-    <sheet name="Table SI 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Table S1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table S2" sheetId="2" r:id="rId2"/>
+    <sheet name="Table S3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table S4" sheetId="4" r:id="rId4"/>
+    <sheet name="Table S5" sheetId="5" r:id="rId5"/>
+    <sheet name="Table S6" sheetId="6" r:id="rId6"/>
+    <sheet name="Table S7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="201">
   <si>
     <t xml:space="preserve">   1.ORI    </t>
   </si>
@@ -141,9 +141,6 @@
     <t>--</t>
   </si>
   <si>
-    <t>Table SI 2. Model selection and log marginal likelihoods obtained from a Bayesian evaluation of temporal signal (BETS) test.</t>
-  </si>
-  <si>
     <t>*0.PRE had temporal signal according to a strict clock, although the relaxed clock with no dates model had the highest likelihood.</t>
   </si>
   <si>
@@ -204,8 +201,584 @@
     <t>Relaxed Clock No Dates*</t>
   </si>
   <si>
+    <t>1.07e-07, 1.49e-07</t>
+  </si>
+  <si>
+    <t>1806, 1901</t>
+  </si>
+  <si>
+    <t>5.81e-08, 1.16e-07</t>
+  </si>
+  <si>
+    <t>1651, 1913</t>
+  </si>
+  <si>
+    <t>4.15e-08, 9.27e-08</t>
+  </si>
+  <si>
+    <t>1655, 1835</t>
+  </si>
+  <si>
+    <t>3.88e-08, 5.71e-08</t>
+  </si>
+  <si>
+    <t>1214, 1315</t>
+  </si>
+  <si>
+    <t>2.01e-07, 2.89e-07</t>
+  </si>
+  <si>
+    <t>1560, 1845</t>
+  </si>
+  <si>
+    <t>5.78e-08, 1.05e-07</t>
+  </si>
+  <si>
+    <t>1509, 1852</t>
+  </si>
+  <si>
+    <t>4.61e-08, 1.52e-07</t>
+  </si>
+  <si>
+    <t>1848, 1968</t>
+  </si>
+  <si>
+    <t>3.69e-08, 1.05e-07</t>
+  </si>
+  <si>
+    <t>1769, 1947</t>
+  </si>
+  <si>
+    <t>2.51e-08, 4.51e-08</t>
+  </si>
+  <si>
+    <t>39, 234</t>
+  </si>
+  <si>
+    <t>4.28e-08, 7.53e-08</t>
+  </si>
+  <si>
+    <t>1357, 1797</t>
+  </si>
+  <si>
+    <t>4.62e-07, 7.68e-07</t>
+  </si>
+  <si>
+    <t>1573, 1876</t>
+  </si>
+  <si>
+    <t>4.15e-08, 6.33e-08</t>
+  </si>
+  <si>
+    <t>-3098, -2786</t>
+  </si>
+  <si>
+    <t>tMRCA</t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t>tMRCA 
+95% HPD</t>
+  </si>
+  <si>
+    <t>Clock Model</t>
+  </si>
+  <si>
+    <t>1.IN*</t>
+  </si>
+  <si>
+    <t>2.ANT*</t>
+  </si>
+  <si>
+    <t>3.ANT*</t>
+  </si>
+  <si>
+    <t>* No temporal signal from the BETS test.</t>
+  </si>
+  <si>
+    <t>1.29e-07, 2.49e-07</t>
+  </si>
+  <si>
+    <t>9.40e-08, 3.17e-07</t>
+  </si>
+  <si>
+    <t>0.00e+00, 1.35e-07</t>
+  </si>
+  <si>
+    <t>6.15e-08, 1.58e-07</t>
+  </si>
+  <si>
+    <t>5.43e-07, 8.83e-07</t>
+  </si>
+  <si>
+    <t>1.35e-07, 4.50e-07</t>
+  </si>
+  <si>
+    <t>8.73e-08, 4.05e-07</t>
+  </si>
+  <si>
+    <t>5.92e-08, 2.95e-07</t>
+  </si>
+  <si>
+    <t>4.77e-08, 1.41e-07</t>
+  </si>
+  <si>
+    <t>7.40e-08, 1.71e-07</t>
+  </si>
+  <si>
+    <t>9.61e-07, 2.10e-06</t>
+  </si>
+  <si>
+    <t>4.75e-08, 1.66e-07</t>
+  </si>
+  <si>
+    <t>Coefficient of Variation</t>
+  </si>
+  <si>
+    <t>Coefficient of Variation
+95% HPD</t>
+  </si>
+  <si>
+    <t>1.09, 1.82</t>
+  </si>
+  <si>
+    <t>1.29, 3.34</t>
+  </si>
+  <si>
+    <t>0.00, 2.12</t>
+  </si>
+  <si>
+    <t>1.38, 3.16</t>
+  </si>
+  <si>
+    <t>2.47, 3.36</t>
+  </si>
+  <si>
+    <t>2.03, 4.95</t>
+  </si>
+  <si>
+    <t>1.43, 3.53</t>
+  </si>
+  <si>
+    <t>1.21, 3.72</t>
+  </si>
+  <si>
+    <t>1.55, 3.83</t>
+  </si>
+  <si>
+    <t>1.49, 2.63</t>
+  </si>
+  <si>
+    <t>1.83, 2.99</t>
+  </si>
+  <si>
+    <t>9.77, 3.07</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>(1) Substitutions / Site / Year</t>
+  </si>
+  <si>
+    <t>(2) Substitutions / Year</t>
+  </si>
+  <si>
+    <t>(3) Years / Substitution</t>
+  </si>
+  <si>
+    <t>1802, 1911</t>
+  </si>
+  <si>
+    <t>1606, 1919</t>
+  </si>
+  <si>
+    <t>1648, 1931</t>
+  </si>
+  <si>
+    <t>662, 1944</t>
+  </si>
+  <si>
+    <t>1645, 1855</t>
+  </si>
+  <si>
+    <t>1323, 1889</t>
+  </si>
+  <si>
+    <t>1208, 1322</t>
+  </si>
+  <si>
+    <t>902, 1329</t>
+  </si>
+  <si>
+    <t>1443, 1874</t>
+  </si>
+  <si>
+    <t>307, 1905</t>
+  </si>
+  <si>
+    <t>1475, 1883</t>
+  </si>
+  <si>
+    <t>317, 1922</t>
+  </si>
+  <si>
+    <t>1847, 1975</t>
+  </si>
+  <si>
+    <t>1516, 1977</t>
+  </si>
+  <si>
+    <t>1769, 1960</t>
+  </si>
+  <si>
+    <t>1145, 1961</t>
+  </si>
+  <si>
+    <t>39, 237</t>
+  </si>
+  <si>
+    <t>-373, 237</t>
+  </si>
+  <si>
+    <t>1349, 1851</t>
+  </si>
+  <si>
+    <t>464, 1941</t>
+  </si>
+  <si>
+    <t>1561, 1906</t>
+  </si>
+  <si>
+    <t>531, 1951</t>
+  </si>
+  <si>
+    <t>-3000, -2777</t>
+  </si>
+  <si>
+    <t>-3408, -2777</t>
+  </si>
+  <si>
+    <t>95% HPD</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>272, 465</t>
+  </si>
+  <si>
+    <t>Continent</t>
+  </si>
+  <si>
+    <t>Samples</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Non-Human Samples</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Same*</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>* Number of samples with a closest relative collected from the same location.</t>
+  </si>
+  <si>
+    <t>Distinct Locations</t>
+  </si>
+  <si>
+    <t>Total Samples</t>
+  </si>
+  <si>
+    <t>MRCA</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Yunnan, China</t>
+  </si>
+  <si>
+    <t>Qinghai, China</t>
+  </si>
+  <si>
+    <t>Nairobi, Kenya</t>
+  </si>
+  <si>
+    <t>Xinjiang, China</t>
+  </si>
+  <si>
+    <t>Inner Mongolia, China</t>
+  </si>
+  <si>
+    <t>Tuva Republic, Russia</t>
+  </si>
+  <si>
+    <t>Issyk-Kul Region, Kyrgzstan</t>
+  </si>
+  <si>
+    <t>Krasnoyarsk Krai, Russia</t>
+  </si>
+  <si>
+    <t>Diverged From</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Table SI 1. </t>
+      <t>1270</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>†</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1800</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>†</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>214</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>†</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>880</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>†</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-2876</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>†</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-1626</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>†</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">† The sampling dates of ancient genomes include the 2-sigma range of radiocarbon estimates. </t>
+  </si>
+  <si>
+    <t>Sampling Time Frame
+(Years)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Pre </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is not a metabolic biovar and refers to "extinct" populations where metabolic status is unknown.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pre*</t>
+  </si>
+  <si>
+    <t>Burnin
+(States)</t>
+  </si>
+  <si>
+    <t>Mean Substitution Rate
+(Substitutions / Site / Year)</t>
+  </si>
+  <si>
+    <t>Mean Substitution Rate 
+95% HPD
+(Substitutions / Site / Year)</t>
+  </si>
+  <si>
+    <t>Substitution Rate
+Standard Deviation
+(Substitutions / Site / Year)</t>
+  </si>
+  <si>
+    <t>Substitution Rate 
+Standard Deviation
+95% HPD
+(Substitutions / Site / Year)</t>
+  </si>
+  <si>
+    <t>0.PRE*</t>
+  </si>
+  <si>
+    <t>* 0.PRE is the most basal population and we could not estimate the divergence location.</t>
+  </si>
+  <si>
+    <t>Tatarstan, Russia</t>
+  </si>
+  <si>
+    <t>95% CI Low</t>
+  </si>
+  <si>
+    <t>95% CI High</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table S1. </t>
     </r>
     <r>
       <rPr>
@@ -230,294 +803,26 @@
     </r>
   </si>
   <si>
-    <t>1.07e-07, 1.49e-07</t>
-  </si>
-  <si>
-    <t>1806, 1901</t>
-  </si>
-  <si>
-    <t>5.81e-08, 1.16e-07</t>
-  </si>
-  <si>
-    <t>1651, 1913</t>
-  </si>
-  <si>
-    <t>4.15e-08, 9.27e-08</t>
-  </si>
-  <si>
-    <t>1655, 1835</t>
-  </si>
-  <si>
-    <t>3.88e-08, 5.71e-08</t>
-  </si>
-  <si>
-    <t>1214, 1315</t>
-  </si>
-  <si>
-    <t>2.01e-07, 2.89e-07</t>
-  </si>
-  <si>
-    <t>1560, 1845</t>
-  </si>
-  <si>
-    <t>5.78e-08, 1.05e-07</t>
-  </si>
-  <si>
-    <t>1509, 1852</t>
-  </si>
-  <si>
-    <t>4.61e-08, 1.52e-07</t>
-  </si>
-  <si>
-    <t>1848, 1968</t>
-  </si>
-  <si>
-    <t>3.69e-08, 1.05e-07</t>
-  </si>
-  <si>
-    <t>1769, 1947</t>
-  </si>
-  <si>
-    <t>2.51e-08, 4.51e-08</t>
-  </si>
-  <si>
-    <t>39, 234</t>
-  </si>
-  <si>
-    <t>4.28e-08, 7.53e-08</t>
-  </si>
-  <si>
-    <t>1357, 1797</t>
-  </si>
-  <si>
-    <t>4.62e-07, 7.68e-07</t>
-  </si>
-  <si>
-    <t>1573, 1876</t>
-  </si>
-  <si>
-    <t>4.15e-08, 6.33e-08</t>
-  </si>
-  <si>
-    <t>-3098, -2786</t>
-  </si>
-  <si>
-    <t>tMRCA</t>
-  </si>
-  <si>
-    <t>States</t>
-  </si>
-  <si>
-    <t>tMRCA 
-95% HPD</t>
-  </si>
-  <si>
-    <t>Clock Model</t>
-  </si>
-  <si>
-    <t>1.IN*</t>
-  </si>
-  <si>
-    <t>2.ANT*</t>
-  </si>
-  <si>
-    <t>3.ANT*</t>
-  </si>
-  <si>
-    <t>* No temporal signal from the BETS test.</t>
-  </si>
-  <si>
-    <t>1.29e-07, 2.49e-07</t>
-  </si>
-  <si>
-    <t>9.40e-08, 3.17e-07</t>
-  </si>
-  <si>
-    <t>0.00e+00, 1.35e-07</t>
-  </si>
-  <si>
-    <t>6.15e-08, 1.58e-07</t>
-  </si>
-  <si>
-    <t>5.43e-07, 8.83e-07</t>
-  </si>
-  <si>
-    <t>1.35e-07, 4.50e-07</t>
-  </si>
-  <si>
-    <t>8.73e-08, 4.05e-07</t>
-  </si>
-  <si>
-    <t>5.92e-08, 2.95e-07</t>
-  </si>
-  <si>
-    <t>4.77e-08, 1.41e-07</t>
-  </si>
-  <si>
-    <t>7.40e-08, 1.71e-07</t>
-  </si>
-  <si>
-    <t>9.61e-07, 2.10e-06</t>
-  </si>
-  <si>
-    <t>4.75e-08, 1.66e-07</t>
-  </si>
-  <si>
-    <t>Coefficient of Variation</t>
-  </si>
-  <si>
-    <t>Coefficient of Variation
-95% HPD</t>
-  </si>
-  <si>
-    <t>1.09, 1.82</t>
-  </si>
-  <si>
-    <t>1.29, 3.34</t>
-  </si>
-  <si>
-    <t>0.00, 2.12</t>
-  </si>
-  <si>
-    <t>1.38, 3.16</t>
-  </si>
-  <si>
-    <t>2.47, 3.36</t>
-  </si>
-  <si>
-    <t>2.03, 4.95</t>
-  </si>
-  <si>
-    <t>1.43, 3.53</t>
-  </si>
-  <si>
-    <t>1.21, 3.72</t>
-  </si>
-  <si>
-    <t>1.55, 3.83</t>
-  </si>
-  <si>
-    <t>1.49, 2.63</t>
-  </si>
-  <si>
-    <t>1.83, 2.99</t>
-  </si>
-  <si>
-    <t>9.77, 3.07</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>Median</t>
-  </si>
-  <si>
-    <t>Standard Deviation</t>
-  </si>
-  <si>
-    <t>(1) Substitutions / Site / Year</t>
-  </si>
-  <si>
-    <t>(2) Substitutions / Year</t>
-  </si>
-  <si>
-    <t>(3) Years / Substitution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table SI 4. Bayesian estimates of the substitution rates by population from the maximum clade credibility (MCC) trees. 
+    <t>Table S2. Model selection and log marginal likelihoods obtained from a Bayesian evaluation of temporal signal (BETS) test.</t>
+  </si>
+  <si>
+    <t>Table S3. Bayesian parameter estimates by population from the Markov chain Monte Carlo (MCMC) analysis. 
+The 95% highest posterior density (HPD) interval indicates the uncertainty surrounding each estimate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table S4. Bayesian estimates of the substitution rates by population from the maximum clade credibility (MCC) trees. 
 Rates are described in units of (1) substitutions per site per year, (2) substitutions per year, and (3) years per substitution based on 4,229,098 genomic sites.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Table SI 5. Bayesian estimates of the time to most recent common ancestor (tMRCA) by population from the maximum clade credibility (MCC) trees. </t>
-  </si>
-  <si>
-    <t>1802, 1911</t>
-  </si>
-  <si>
-    <t>1606, 1919</t>
-  </si>
-  <si>
-    <t>1648, 1931</t>
-  </si>
-  <si>
-    <t>662, 1944</t>
-  </si>
-  <si>
-    <t>1645, 1855</t>
-  </si>
-  <si>
-    <t>1323, 1889</t>
-  </si>
-  <si>
-    <t>1208, 1322</t>
-  </si>
-  <si>
-    <t>902, 1329</t>
-  </si>
-  <si>
-    <t>1443, 1874</t>
-  </si>
-  <si>
-    <t>307, 1905</t>
-  </si>
-  <si>
-    <t>1475, 1883</t>
-  </si>
-  <si>
-    <t>317, 1922</t>
-  </si>
-  <si>
-    <t>1847, 1975</t>
-  </si>
-  <si>
-    <t>1516, 1977</t>
-  </si>
-  <si>
-    <t>1769, 1960</t>
-  </si>
-  <si>
-    <t>1145, 1961</t>
-  </si>
-  <si>
-    <t>39, 237</t>
-  </si>
-  <si>
-    <t>-373, 237</t>
-  </si>
-  <si>
-    <t>1349, 1851</t>
-  </si>
-  <si>
-    <t>464, 1941</t>
-  </si>
-  <si>
-    <t>1561, 1906</t>
-  </si>
-  <si>
-    <t>531, 1951</t>
-  </si>
-  <si>
-    <t>-3000, -2777</t>
-  </si>
-  <si>
-    <t>-3408, -2777</t>
-  </si>
-  <si>
-    <t>95% HPD</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>First Pandemic Clade</t>
-  </si>
-  <si>
-    <t>272, 465</t>
+    <t xml:space="preserve">Table S5. Bayesian estimates of the time to most recent common ancestor (tMRCA) by population from the maximum clade credibility (MCC) trees. </t>
+  </si>
+  <si>
+    <t>First Pandemic MRCA</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Table SI 6. Geographic structure of </t>
+      <t xml:space="preserve">Table S6. Geographic structure of </t>
     </r>
     <r>
       <rPr>
@@ -538,316 +843,11 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> populations.</t>
+      <t xml:space="preserve"> populations according to the number of samples with a closest relative collected from the same location.</t>
     </r>
   </si>
   <si>
-    <t>Continent</t>
-  </si>
-  <si>
-    <t>Samples</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Non-Human Samples</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>Same*</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>* Number of samples with a closest relative collected from the same location.</t>
-  </si>
-  <si>
-    <t>Distinct Locations</t>
-  </si>
-  <si>
-    <t>Total Samples</t>
-  </si>
-  <si>
-    <t>MRCA</t>
-  </si>
-  <si>
-    <t>Confidence</t>
-  </si>
-  <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Africa</t>
-  </si>
-  <si>
-    <t>Europe</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Kenya</t>
-  </si>
-  <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>Kyrgyzstan</t>
-  </si>
-  <si>
-    <t>Yunnan, China</t>
-  </si>
-  <si>
-    <t>Qinghai, China</t>
-  </si>
-  <si>
-    <t>Nairobi, Kenya</t>
-  </si>
-  <si>
-    <t>Xinjiang, China</t>
-  </si>
-  <si>
-    <t>Inner Mongolia, China</t>
-  </si>
-  <si>
-    <t>Tuva Republic, Russia</t>
-  </si>
-  <si>
-    <t>Issyk-Kul Region, Kyrgzstan</t>
-  </si>
-  <si>
-    <t>Krasnoyarsk Krai, Russia</t>
-  </si>
-  <si>
-    <t>Diverged From</t>
-  </si>
-  <si>
-    <t>Table SI 7. Ancestral location estimation.</t>
-  </si>
-  <si>
-    <r>
-      <t>1270</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1800</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>214</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>880</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-2876</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>-1626</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>†</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">† The sampling dates of ancient genomes include the 2-sigma range of radiocarbon estimates. </t>
-  </si>
-  <si>
-    <t>Sampling Time Frame
-(Years)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">* </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Pre </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>is not a metabolic biovar and refers to "extinct" populations where metabolic status is unknown.</t>
-    </r>
-  </si>
-  <si>
-    <t>Pre*</t>
-  </si>
-  <si>
-    <t>Burnin
-(States)</t>
-  </si>
-  <si>
-    <t>Mean Substitution Rate
-(Substitutions / Site / Year)</t>
-  </si>
-  <si>
-    <t>Mean Substitution Rate 
-95% HPD
-(Substitutions / Site / Year)</t>
-  </si>
-  <si>
-    <t>Substitution Rate
-Standard Deviation
-(Substitutions / Site / Year)</t>
-  </si>
-  <si>
-    <t>Substitution Rate 
-Standard Deviation
-95% HPD
-(Substitutions / Site / Year)</t>
-  </si>
-  <si>
-    <t>Table SI 3. Bayesian parameter estimates by population from the Markov chain Monte Carlo (MCMC) analysis. 
-The 95% highest posterior density (HPD) interval indicates the uncertainty surrounding each estimate.</t>
-  </si>
-  <si>
-    <t>0.PRE*</t>
-  </si>
-  <si>
-    <t>* 0.PRE is the most basal population and we could not estimate the divergence location.</t>
-  </si>
-  <si>
-    <t>Tatarstan, Russia</t>
-  </si>
-  <si>
-    <t>95% CI Low</t>
-  </si>
-  <si>
-    <t>95% CI High</t>
+    <t>Table S7. Ancestral location estimation by independently fitting three discrete migration models to the maximum likelihood phylogeny using the sampling locations by: (1) continent, (2) country, and (3) province.</t>
   </si>
 </sst>
 </file>
@@ -1044,12 +1044,11 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1238,12 +1237,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC9C9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1716,7 +1709,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1945,42 +1938,6 @@
     <xf numFmtId="0" fontId="20" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2015,38 +1972,11 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2087,6 +2017,57 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="25" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2451,7 +2432,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2468,17 +2449,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="89.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="116" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
+      <c r="A1" s="95" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -2503,7 +2484,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>23</v>
@@ -2607,7 +2588,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -2616,10 +2597,10 @@
         <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H6" s="41">
         <f>1800-1270</f>
@@ -2766,10 +2747,10 @@
         <v>12</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H11" s="41">
         <f>880-214</f>
@@ -2847,7 +2828,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="D14" s="8">
         <v>0</v>
@@ -2856,10 +2837,10 @@
         <v>8</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H14" s="42">
         <f>2876-1626</f>
@@ -2871,7 +2852,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -2884,7 +2865,7 @@
     </row>
     <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -2912,7 +2893,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2929,41 +2910,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="120"/>
+      <c r="A1" s="97" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="99"/>
     </row>
     <row r="2" spans="1:8" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2974,7 +2955,7 @@
         <v>117</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="43">
         <f>H3-G3</f>
@@ -2995,13 +2976,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="35">
         <v>39</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="44">
         <f t="shared" ref="D4:D14" si="0">H4-G4</f>
@@ -3022,13 +3003,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="35">
         <v>4</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="44">
         <f t="shared" si="0"/>
@@ -3049,13 +3030,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="35">
         <v>40</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" s="44">
         <f t="shared" si="0"/>
@@ -3076,13 +3057,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="35">
         <v>116</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="44">
         <f t="shared" si="0"/>
@@ -3103,13 +3084,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="35">
         <v>54</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="44">
         <f t="shared" si="0"/>
@@ -3130,13 +3111,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="35">
         <v>11</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="44">
         <f t="shared" si="0"/>
@@ -3157,13 +3138,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="35">
         <v>11</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="44">
         <f t="shared" si="0"/>
@@ -3184,13 +3165,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="35">
         <v>12</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="44">
         <f t="shared" si="0"/>
@@ -3211,13 +3192,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="35">
         <v>103</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" s="44">
         <f t="shared" si="0"/>
@@ -3238,13 +3219,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="35">
         <v>85</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="44">
         <f t="shared" si="0"/>
@@ -3265,13 +3246,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="36">
         <v>8</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" s="48">
         <f t="shared" si="0"/>
@@ -3292,7 +3273,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -3314,8 +3295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3336,15 +3317,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="95" t="s">
         <v>195</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
       <c r="H1" s="56"/>
       <c r="I1" s="56"/>
       <c r="J1" s="56"/>
@@ -3356,37 +3337,37 @@
         <v>30</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E2" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="50" t="s">
-        <v>82</v>
-      </c>
       <c r="G2" s="50" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="H2" s="50" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J2" s="50" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K2" s="50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L2" s="50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
@@ -3394,7 +3375,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="35">
         <v>143600000</v>
@@ -3407,33 +3388,33 @@
         <v>1866.83908296345</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G3" s="52">
         <v>1.29E-7</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I3" s="52">
         <v>1.66E-7</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K3" s="53">
         <v>1.38</v>
       </c>
       <c r="L3" s="53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" s="35">
         <v>1000000000</v>
@@ -3446,33 +3427,33 @@
         <v>1824.6353683781499</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G4" s="52">
         <v>8.6599999999999995E-8</v>
       </c>
       <c r="H4" s="35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I4" s="52">
         <v>1.6E-7</v>
       </c>
       <c r="J4" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K4" s="53">
         <v>2.15</v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="35">
         <v>1000000000</v>
@@ -3485,33 +3466,33 @@
         <v>1759.0973808542799</v>
       </c>
       <c r="F5" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" s="52">
         <v>6.4799999999999998E-8</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I5" s="52">
         <v>-1.0499999999999999E-11</v>
       </c>
       <c r="J5" s="35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K5" s="53">
         <v>0.47899999999999998</v>
       </c>
       <c r="L5" s="53" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="35">
         <v>426000000</v>
@@ -3524,33 +3505,33 @@
         <v>1278.8596741967499</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G6" s="52">
         <v>4.7699999999999997E-8</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I6" s="52">
         <v>8.5899999999999995E-8</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K6" s="53">
         <v>2.06</v>
       </c>
       <c r="L6" s="53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="35">
         <v>371100000</v>
@@ -3563,33 +3544,33 @@
         <v>1744.3012451940699</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" s="52">
         <v>2.4600000000000001E-7</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I7" s="52">
         <v>6.8700000000000005E-7</v>
       </c>
       <c r="J7" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K7" s="53">
         <v>2.86</v>
       </c>
       <c r="L7" s="53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="35">
         <v>1000000000</v>
@@ -3602,33 +3583,33 @@
         <v>1730.63967066134</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G8" s="52">
         <v>8.0799999999999996E-8</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I8" s="52">
         <v>2.3099999999999999E-7</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K8" s="53">
         <v>3.29</v>
       </c>
       <c r="L8" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="35">
         <v>1000000000</v>
@@ -3641,33 +3622,33 @@
         <v>1927.2701397952001</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G9" s="52">
         <v>9.3800000000000006E-8</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I9" s="52">
         <v>1.6500000000000001E-7</v>
       </c>
       <c r="J9" s="35" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K9" s="53">
         <v>2.27</v>
       </c>
       <c r="L9" s="53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="35">
         <v>1000000000</v>
@@ -3680,33 +3661,33 @@
         <v>1885.2057410805301</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G10" s="52">
         <v>6.8799999999999994E-8</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I10" s="52">
         <v>1.1300000000000001E-7</v>
       </c>
       <c r="J10" s="35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K10" s="53">
         <v>2.1800000000000002</v>
       </c>
       <c r="L10" s="53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="35">
         <v>1000000000</v>
@@ -3719,33 +3700,33 @@
         <v>172.63238860707401</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="52">
         <v>3.5100000000000003E-8</v>
       </c>
       <c r="H11" s="35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" s="52">
         <v>7.2499999999999994E-8</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K11" s="53">
         <v>2.4900000000000002</v>
       </c>
       <c r="L11" s="53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="35">
         <v>1000000000</v>
@@ -3758,33 +3739,33 @@
         <v>1627.8309293028799</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G12" s="52">
         <v>5.8500000000000001E-8</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I12" s="52">
         <v>1.03E-7</v>
       </c>
       <c r="J12" s="35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K12" s="53">
         <v>1.96</v>
       </c>
       <c r="L12" s="53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="35">
         <v>443400000</v>
@@ -3797,33 +3778,33 @@
         <v>1763.58649732858</v>
       </c>
       <c r="F13" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G13" s="52">
         <v>6.1500000000000004E-7</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I13" s="52">
         <v>1.3E-6</v>
       </c>
       <c r="J13" s="35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K13" s="53">
         <v>2.29</v>
       </c>
       <c r="L13" s="53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="36">
         <v>5000000000</v>
@@ -3836,30 +3817,30 @@
         <v>-2891.8793123557998</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G14" s="54">
         <v>5.2999999999999998E-8</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I14" s="54">
         <v>7.2699999999999996E-8</v>
       </c>
       <c r="J14" s="36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K14" s="55">
         <v>1.74</v>
       </c>
       <c r="L14" s="55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -3875,65 +3856,65 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="G16" s="10"/>
-      <c r="K16" s="115"/>
+      <c r="K16" s="94"/>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.35">
       <c r="G17" s="10"/>
-      <c r="K17" s="115"/>
+      <c r="K17" s="94"/>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.35">
       <c r="G18" s="10"/>
-      <c r="K18" s="115"/>
+      <c r="K18" s="94"/>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="K19" s="115"/>
+      <c r="K19" s="94"/>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D20" s="10"/>
       <c r="G20" s="10"/>
-      <c r="K20" s="115"/>
+      <c r="K20" s="94"/>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D21" s="10"/>
       <c r="G21" s="10"/>
-      <c r="K21" s="115"/>
+      <c r="K21" s="94"/>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="K22" s="115"/>
+      <c r="K22" s="94"/>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D23" s="10"/>
       <c r="G23" s="10"/>
-      <c r="K23" s="115"/>
+      <c r="K23" s="94"/>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D24" s="10"/>
       <c r="G24" s="10"/>
-      <c r="K24" s="115"/>
+      <c r="K24" s="94"/>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D25" s="10"/>
       <c r="G25" s="10"/>
-      <c r="K25" s="115"/>
+      <c r="K25" s="94"/>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D26" s="10"/>
       <c r="G26" s="10"/>
-      <c r="K26" s="115"/>
+      <c r="K26" s="94"/>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D27" s="10"/>
       <c r="G27" s="10"/>
-      <c r="K27" s="115"/>
+      <c r="K27" s="94"/>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D28" s="10"/>
       <c r="G28" s="10"/>
-      <c r="K28" s="115"/>
+      <c r="K28" s="94"/>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D29" s="10"/>
@@ -3957,7 +3938,7 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3978,97 +3959,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="124" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="126"/>
+      <c r="A1" s="103" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="104"/>
+      <c r="I1" s="104"/>
+      <c r="J1" s="104"/>
+      <c r="K1" s="104"/>
+      <c r="L1" s="104"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="104"/>
+      <c r="O1" s="104"/>
+      <c r="P1" s="105"/>
     </row>
     <row r="2" spans="1:23" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="100" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="100" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="121" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="121" t="s">
-        <v>119</v>
-      </c>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="123"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="102"/>
     </row>
     <row r="3" spans="1:23" ht="59.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="57" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="F3" s="60" t="s">
-        <v>116</v>
-      </c>
       <c r="G3" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="J3" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="60" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="J3" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="K3" s="60" t="s">
-        <v>116</v>
-      </c>
       <c r="L3" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="O3" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="P3" s="60" t="s">
         <v>114</v>
-      </c>
-      <c r="M3" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="N3" s="59" t="s">
-        <v>199</v>
-      </c>
-      <c r="O3" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="P3" s="60" t="s">
-        <v>116</v>
       </c>
       <c r="Q3" s="61"/>
       <c r="R3" s="61"/>
@@ -4139,7 +4120,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="65">
         <v>8.9201527841334796E-8</v>
@@ -4198,7 +4179,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="65">
         <v>5.5556110260483602E-8</v>
@@ -4257,7 +4238,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="65">
         <v>5.1097666695877699E-8</v>
@@ -4316,7 +4297,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="65">
         <v>3.4498430728329802E-7</v>
@@ -4375,7 +4356,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="62" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B9" s="65">
         <v>1.00518867433374E-7</v>
@@ -4434,7 +4415,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="65">
         <v>1.3086924358689199E-7</v>
@@ -4493,7 +4474,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="62" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="65">
         <v>1.5357687690296499E-7</v>
@@ -4552,7 +4533,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="65">
         <v>6.8983168049580905E-8</v>
@@ -4611,7 +4592,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="65">
         <v>3.5823293194635201E-8</v>
@@ -4670,7 +4651,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="65">
         <v>8.62945505677659E-7</v>
@@ -4729,7 +4710,7 @@
     </row>
     <row r="15" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="71">
         <v>8.1161224199588901E-8</v>
@@ -4788,7 +4769,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="51" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="11:11" x14ac:dyDescent="0.35">
@@ -4842,13 +4823,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F63E50-22E0-4F4B-BE73-D5E646308EF9}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="1" max="1" width="35.26953125" customWidth="1"/>
     <col min="2" max="2" width="16.453125" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="25.7265625" customWidth="1"/>
@@ -4856,287 +4837,292 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="124" t="s">
-        <v>121</v>
-      </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
+      <c r="A1" s="103" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
     </row>
     <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
-      <c r="B2" s="121" t="s">
-        <v>80</v>
-      </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="123"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
+      <c r="B2" s="100" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="102"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
     </row>
     <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="57" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C3" s="78" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D3" s="78" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E3" s="79" t="s">
-        <v>147</v>
-      </c>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
+        <v>143</v>
+      </c>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
     </row>
     <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="109">
         <v>1867</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="110">
         <v>1875</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="110" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="111" t="s">
+        <v>119</v>
+      </c>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="108" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="109">
+        <v>1825</v>
+      </c>
+      <c r="C5" s="110">
+        <v>1849</v>
+      </c>
+      <c r="D5" s="110" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="111" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="109">
+        <v>1759</v>
+      </c>
+      <c r="C6" s="110">
+        <v>1767</v>
+      </c>
+      <c r="D6" s="110" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="84" t="s">
+      <c r="E6" s="111" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="80" t="s">
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="109">
+        <v>1279</v>
+      </c>
+      <c r="C7" s="110">
+        <v>1287</v>
+      </c>
+      <c r="D7" s="110" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="111" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="81"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="108" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="109">
+        <v>1713</v>
+      </c>
+      <c r="C8" s="110">
+        <v>1750</v>
+      </c>
+      <c r="D8" s="110" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="108" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="109">
+        <v>1723</v>
+      </c>
+      <c r="C9" s="110">
+        <v>1756</v>
+      </c>
+      <c r="D9" s="110" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" s="111" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="108" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="109">
+        <v>1927</v>
+      </c>
+      <c r="C10" s="110">
+        <v>1938</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="111" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="85">
-        <v>1825</v>
-      </c>
-      <c r="C5" s="86">
-        <v>1849</v>
-      </c>
-      <c r="D5" s="86" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" s="87" t="s">
-        <v>125</v>
-      </c>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="82">
-        <v>1759</v>
-      </c>
-      <c r="C6" s="83">
+      <c r="B11" s="109">
+        <v>1885</v>
+      </c>
+      <c r="C11" s="110">
+        <v>1902</v>
+      </c>
+      <c r="D11" s="110" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="111" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="108" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="109">
+        <v>173</v>
+      </c>
+      <c r="C12" s="110">
+        <v>195</v>
+      </c>
+      <c r="D12" s="110" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="111" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" s="109">
+        <v>386</v>
+      </c>
+      <c r="C13" s="110">
+        <v>399</v>
+      </c>
+      <c r="D13" s="110" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="112">
+        <v>40474</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="108" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="109">
+        <v>1629</v>
+      </c>
+      <c r="C14" s="110">
+        <v>1658</v>
+      </c>
+      <c r="D14" s="110" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="111" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="108" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="109">
         <v>1767</v>
       </c>
-      <c r="D6" s="83" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="84" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="82">
-        <v>1279</v>
-      </c>
-      <c r="C7" s="83">
-        <v>1287</v>
-      </c>
-      <c r="D7" s="83" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="84" t="s">
-        <v>129</v>
-      </c>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="82">
-        <v>1713</v>
-      </c>
-      <c r="C8" s="83">
-        <v>1750</v>
-      </c>
-      <c r="D8" s="83" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="84" t="s">
-        <v>131</v>
-      </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="80" t="s">
+      <c r="C15" s="110">
+        <v>1790</v>
+      </c>
+      <c r="D15" s="110" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="111" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="113" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="114">
+        <v>-2852</v>
+      </c>
+      <c r="C16" s="115">
+        <v>-2829</v>
+      </c>
+      <c r="D16" s="115" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" s="116" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="51" t="s">
         <v>85</v>
-      </c>
-      <c r="B9" s="85">
-        <v>1723</v>
-      </c>
-      <c r="C9" s="86">
-        <v>1756</v>
-      </c>
-      <c r="D9" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="87" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="62" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="82">
-        <v>1927</v>
-      </c>
-      <c r="C10" s="83">
-        <v>1938</v>
-      </c>
-      <c r="D10" s="83" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="84" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="80" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="85">
-        <v>1885</v>
-      </c>
-      <c r="C11" s="86">
-        <v>1902</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="87" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="82">
-        <v>173</v>
-      </c>
-      <c r="C12" s="83">
-        <v>195</v>
-      </c>
-      <c r="D12" s="83" t="s">
-        <v>138</v>
-      </c>
-      <c r="E12" s="84" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="81" t="s">
-        <v>148</v>
-      </c>
-      <c r="B13" s="82">
-        <v>386</v>
-      </c>
-      <c r="C13" s="83">
-        <v>399</v>
-      </c>
-      <c r="D13" s="83" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="88">
-        <v>40474</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="82">
-        <v>1629</v>
-      </c>
-      <c r="C14" s="83">
-        <v>1658</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="84" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="82">
-        <v>1767</v>
-      </c>
-      <c r="C15" s="83">
-        <v>1790</v>
-      </c>
-      <c r="D15" s="83" t="s">
-        <v>142</v>
-      </c>
-      <c r="E15" s="84" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" s="89">
-        <v>-2852</v>
-      </c>
-      <c r="C16" s="90">
-        <v>-2829</v>
-      </c>
-      <c r="D16" s="90" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16" s="91" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
@@ -5157,8 +5143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922555F0-DD60-4A30-94C9-BFE9FAE6D9F6}">
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5169,92 +5155,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="127" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
+      <c r="A1" s="106" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
     </row>
     <row r="2" spans="1:15" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="15"/>
-      <c r="D2" s="121" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="121" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="123"/>
+      <c r="D2" s="100" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="100" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="101"/>
+      <c r="N2" s="101"/>
+      <c r="O2" s="102"/>
     </row>
     <row r="3" spans="1:15" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="J3" s="28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K3" s="31" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="N3" s="28" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O3" s="31" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -5306,7 +5292,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="21">
         <v>39</v>
@@ -5353,7 +5339,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="21">
         <v>4</v>
@@ -5385,22 +5371,22 @@
       <c r="K6" s="22">
         <v>50</v>
       </c>
-      <c r="L6" s="94">
+      <c r="L6" s="82">
         <v>1</v>
       </c>
-      <c r="M6" s="95">
+      <c r="M6" s="83">
         <v>1</v>
       </c>
-      <c r="N6" s="96">
+      <c r="N6" s="84">
         <v>0</v>
       </c>
-      <c r="O6" s="97">
+      <c r="O6" s="85">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="21">
         <v>40</v>
@@ -5447,7 +5433,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="21">
         <v>116</v>
@@ -5494,7 +5480,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" s="21">
         <v>54</v>
@@ -5541,7 +5527,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="21">
         <v>11</v>
@@ -5588,7 +5574,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="21">
         <v>11</v>
@@ -5635,7 +5621,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="21">
         <v>12</v>
@@ -5682,7 +5668,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="21">
         <v>103</v>
@@ -5729,7 +5715,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="21">
         <v>86</v>
@@ -5776,7 +5762,7 @@
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="18">
         <v>8</v>
@@ -5823,7 +5809,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -5843,7 +5829,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5864,620 +5850,620 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="127" t="s">
-        <v>179</v>
-      </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
+      <c r="A1" s="106" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
     </row>
     <row r="2" spans="1:14" ht="65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="121" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="121" t="s">
-        <v>153</v>
-      </c>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="121" t="s">
+      <c r="C2" s="100" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="100" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="L2" s="101"/>
+      <c r="M2" s="101"/>
+      <c r="N2" s="102"/>
+    </row>
+    <row r="3" spans="1:14" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="87" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="77" t="s">
         <v>155</v>
       </c>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="123"/>
-    </row>
-    <row r="3" spans="1:14" s="16" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="99" t="s">
+      <c r="D3" s="88" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="77" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="88" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="J3" s="79" t="s">
+        <v>156</v>
+      </c>
+      <c r="K3" s="77" t="s">
+        <v>155</v>
+      </c>
+      <c r="L3" s="88" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" s="89" t="s">
+        <v>172</v>
+      </c>
+      <c r="N3" s="79" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="91">
+        <v>117</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="117">
+        <v>100</v>
+      </c>
+      <c r="E4" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="119">
+        <v>100</v>
+      </c>
+      <c r="G4" s="120" t="s">
         <v>160</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="H4" s="117">
+        <v>100</v>
+      </c>
+      <c r="I4" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J4" s="119">
+        <v>100</v>
+      </c>
+      <c r="K4" s="120" t="s">
+        <v>164</v>
+      </c>
+      <c r="L4" s="117">
+        <v>99</v>
+      </c>
+      <c r="M4" s="118" t="s">
+        <v>164</v>
+      </c>
+      <c r="N4" s="119">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="91">
+        <v>39</v>
+      </c>
+      <c r="C5" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="117">
+        <v>100</v>
+      </c>
+      <c r="E5" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="119">
+        <v>63</v>
+      </c>
+      <c r="G5" s="120" t="s">
+        <v>160</v>
+      </c>
+      <c r="H5" s="117">
+        <v>100</v>
+      </c>
+      <c r="I5" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J5" s="119">
+        <v>41</v>
+      </c>
+      <c r="K5" s="120" t="s">
+        <v>165</v>
+      </c>
+      <c r="L5" s="117">
+        <v>100</v>
+      </c>
+      <c r="M5" s="118" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="119">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="91">
+        <v>4</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="117">
+        <v>100</v>
+      </c>
+      <c r="E6" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="119">
+        <v>63</v>
+      </c>
+      <c r="G6" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="H6" s="117">
+        <v>44</v>
+      </c>
+      <c r="I6" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" s="119">
+        <v>41</v>
+      </c>
+      <c r="K6" s="120" t="s">
+        <v>166</v>
+      </c>
+      <c r="L6" s="117">
+        <v>56</v>
+      </c>
+      <c r="M6" s="118" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" s="119">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="90" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="91">
+        <v>40</v>
+      </c>
+      <c r="C7" s="90" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="117">
+        <v>98</v>
+      </c>
+      <c r="E7" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="119">
+        <v>91</v>
+      </c>
+      <c r="G7" s="120" t="s">
         <v>162</v>
       </c>
-      <c r="E3" s="101" t="s">
-        <v>178</v>
-      </c>
-      <c r="F3" s="79" t="s">
+      <c r="H7" s="117">
+        <v>63</v>
+      </c>
+      <c r="I7" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J7" s="119">
+        <v>93</v>
+      </c>
+      <c r="K7" s="120" t="s">
+        <v>190</v>
+      </c>
+      <c r="L7" s="117">
+        <v>37</v>
+      </c>
+      <c r="M7" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="N7" s="119">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="91">
+        <v>116</v>
+      </c>
+      <c r="C8" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D8" s="117">
+        <v>92</v>
+      </c>
+      <c r="E8" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="119">
+        <v>95</v>
+      </c>
+      <c r="G8" s="120" t="s">
+        <v>160</v>
+      </c>
+      <c r="H8" s="117">
+        <v>94</v>
+      </c>
+      <c r="I8" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J8" s="119">
+        <v>96</v>
+      </c>
+      <c r="K8" s="120" t="s">
+        <v>167</v>
+      </c>
+      <c r="L8" s="117">
+        <v>59</v>
+      </c>
+      <c r="M8" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="N8" s="119">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="91">
+        <v>54</v>
+      </c>
+      <c r="C9" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" s="117">
+        <v>100</v>
+      </c>
+      <c r="E9" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="119">
+        <v>95</v>
+      </c>
+      <c r="G9" s="120" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" s="117">
+        <v>100</v>
+      </c>
+      <c r="I9" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J9" s="119">
+        <v>96</v>
+      </c>
+      <c r="K9" s="120" t="s">
+        <v>168</v>
+      </c>
+      <c r="L9" s="117">
+        <v>50</v>
+      </c>
+      <c r="M9" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="N9" s="119">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="91">
+        <v>11</v>
+      </c>
+      <c r="C10" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D10" s="117">
+        <v>59</v>
+      </c>
+      <c r="E10" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="119">
+        <v>96</v>
+      </c>
+      <c r="G10" s="120" t="s">
         <v>162</v>
       </c>
-      <c r="G3" s="77" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" s="100" t="s">
+      <c r="H10" s="117">
+        <v>97</v>
+      </c>
+      <c r="I10" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J10" s="119">
+        <v>92</v>
+      </c>
+      <c r="K10" s="120" t="s">
+        <v>169</v>
+      </c>
+      <c r="L10" s="117">
+        <v>68</v>
+      </c>
+      <c r="M10" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="N10" s="119">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="91">
+        <v>11</v>
+      </c>
+      <c r="C11" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="117">
+        <v>100</v>
+      </c>
+      <c r="E11" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="119">
+        <v>96</v>
+      </c>
+      <c r="G11" s="120" t="s">
+        <v>160</v>
+      </c>
+      <c r="H11" s="117">
+        <v>95</v>
+      </c>
+      <c r="I11" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" s="119">
+        <v>92</v>
+      </c>
+      <c r="K11" s="120" t="s">
+        <v>165</v>
+      </c>
+      <c r="L11" s="117">
+        <v>32</v>
+      </c>
+      <c r="M11" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="N11" s="119">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="90" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="91">
+        <v>12</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="117">
+        <v>97</v>
+      </c>
+      <c r="E12" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="119">
+        <v>100</v>
+      </c>
+      <c r="G12" s="120" t="s">
+        <v>163</v>
+      </c>
+      <c r="H12" s="117">
+        <v>69</v>
+      </c>
+      <c r="I12" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J12" s="119">
+        <v>57</v>
+      </c>
+      <c r="K12" s="120" t="s">
+        <v>170</v>
+      </c>
+      <c r="L12" s="117">
+        <v>71</v>
+      </c>
+      <c r="M12" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="N12" s="119">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="90" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="91">
+        <v>103</v>
+      </c>
+      <c r="C13" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="117">
+        <v>100</v>
+      </c>
+      <c r="E13" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13" s="119">
+        <v>100</v>
+      </c>
+      <c r="G13" s="120" t="s">
+        <v>160</v>
+      </c>
+      <c r="H13" s="117">
+        <v>92</v>
+      </c>
+      <c r="I13" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="119">
+        <v>64</v>
+      </c>
+      <c r="K13" s="120" t="s">
+        <v>167</v>
+      </c>
+      <c r="L13" s="117">
+        <v>76</v>
+      </c>
+      <c r="M13" s="118" t="s">
+        <v>165</v>
+      </c>
+      <c r="N13" s="119">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="90" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="91">
+        <v>86</v>
+      </c>
+      <c r="C14" s="90" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="117">
+        <v>94</v>
+      </c>
+      <c r="E14" s="118" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14" s="119">
+        <v>52</v>
+      </c>
+      <c r="G14" s="120" t="s">
         <v>162</v>
       </c>
-      <c r="I3" s="101" t="s">
-        <v>178</v>
-      </c>
-      <c r="J3" s="79" t="s">
+      <c r="H14" s="117">
+        <v>71</v>
+      </c>
+      <c r="I14" s="118" t="s">
         <v>162</v>
       </c>
-      <c r="K3" s="77" t="s">
-        <v>161</v>
-      </c>
-      <c r="L3" s="100" t="s">
-        <v>162</v>
-      </c>
-      <c r="M3" s="101" t="s">
-        <v>178</v>
-      </c>
-      <c r="N3" s="79" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="102" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="103">
-        <v>117</v>
-      </c>
-      <c r="C4" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D4" s="104">
-        <v>100</v>
-      </c>
-      <c r="E4" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F4" s="106">
-        <v>100</v>
-      </c>
-      <c r="G4" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H4" s="104">
-        <v>100</v>
-      </c>
-      <c r="I4" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J4" s="106">
-        <v>100</v>
-      </c>
-      <c r="K4" s="102" t="s">
-        <v>170</v>
-      </c>
-      <c r="L4" s="104">
+      <c r="J14" s="119">
+        <v>85</v>
+      </c>
+      <c r="K14" s="120" t="s">
+        <v>165</v>
+      </c>
+      <c r="L14" s="117">
         <v>99</v>
       </c>
-      <c r="M4" s="105" t="s">
-        <v>170</v>
-      </c>
-      <c r="N4" s="106">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="102" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="103">
-        <v>39</v>
-      </c>
-      <c r="C5" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="104">
-        <v>100</v>
-      </c>
-      <c r="E5" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" s="113">
-        <v>63</v>
-      </c>
-      <c r="G5" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H5" s="104">
-        <v>100</v>
-      </c>
-      <c r="I5" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J5" s="113">
-        <v>41</v>
-      </c>
-      <c r="K5" s="102" t="s">
-        <v>171</v>
-      </c>
-      <c r="L5" s="104">
-        <v>100</v>
-      </c>
-      <c r="M5" s="105" t="s">
-        <v>171</v>
-      </c>
-      <c r="N5" s="113">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="102" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="103">
-        <v>4</v>
-      </c>
-      <c r="C6" s="102" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="104">
-        <v>100</v>
-      </c>
-      <c r="E6" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F6" s="113">
-        <v>63</v>
-      </c>
-      <c r="G6" s="102" t="s">
-        <v>167</v>
-      </c>
-      <c r="H6" s="112">
-        <v>44</v>
-      </c>
-      <c r="I6" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J6" s="113">
-        <v>41</v>
-      </c>
-      <c r="K6" s="102" t="s">
-        <v>172</v>
-      </c>
-      <c r="L6" s="112">
-        <v>56</v>
-      </c>
-      <c r="M6" s="105" t="s">
-        <v>171</v>
-      </c>
-      <c r="N6" s="113">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="102" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="103">
-        <v>40</v>
-      </c>
-      <c r="C7" s="102" t="s">
+      <c r="M14" s="118" t="s">
         <v>165</v>
       </c>
-      <c r="D7" s="104">
-        <v>98</v>
-      </c>
-      <c r="E7" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F7" s="106">
-        <v>91</v>
-      </c>
-      <c r="G7" s="102" t="s">
-        <v>168</v>
-      </c>
-      <c r="H7" s="112">
-        <v>63</v>
-      </c>
-      <c r="I7" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J7" s="106">
-        <v>93</v>
-      </c>
-      <c r="K7" s="102" t="s">
-        <v>198</v>
-      </c>
-      <c r="L7" s="112">
-        <v>37</v>
-      </c>
-      <c r="M7" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="N7" s="113">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="102" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="103">
-        <v>116</v>
-      </c>
-      <c r="C8" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D8" s="104">
-        <v>92</v>
-      </c>
-      <c r="E8" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F8" s="106">
-        <v>95</v>
-      </c>
-      <c r="G8" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H8" s="104">
-        <v>94</v>
-      </c>
-      <c r="I8" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J8" s="106">
-        <v>96</v>
-      </c>
-      <c r="K8" s="102" t="s">
-        <v>173</v>
-      </c>
-      <c r="L8" s="112">
-        <v>59</v>
-      </c>
-      <c r="M8" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="N8" s="113">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="102" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="103">
-        <v>54</v>
-      </c>
-      <c r="C9" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D9" s="104">
-        <v>100</v>
-      </c>
-      <c r="E9" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F9" s="106">
-        <v>95</v>
-      </c>
-      <c r="G9" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H9" s="104">
-        <v>100</v>
-      </c>
-      <c r="I9" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J9" s="106">
-        <v>96</v>
-      </c>
-      <c r="K9" s="102" t="s">
-        <v>174</v>
-      </c>
-      <c r="L9" s="112">
-        <v>50</v>
-      </c>
-      <c r="M9" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="N9" s="113">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="102" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="103">
-        <v>11</v>
-      </c>
-      <c r="C10" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D10" s="112">
-        <v>59</v>
-      </c>
-      <c r="E10" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F10" s="106">
-        <v>96</v>
-      </c>
-      <c r="G10" s="102" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" s="104">
-        <v>97</v>
-      </c>
-      <c r="I10" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J10" s="106">
-        <v>92</v>
-      </c>
-      <c r="K10" s="102" t="s">
-        <v>175</v>
-      </c>
-      <c r="L10" s="112">
-        <v>68</v>
-      </c>
-      <c r="M10" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="N10" s="113">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="102" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="103">
-        <v>11</v>
-      </c>
-      <c r="C11" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="104">
-        <v>100</v>
-      </c>
-      <c r="E11" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F11" s="106">
-        <v>96</v>
-      </c>
-      <c r="G11" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H11" s="104">
-        <v>95</v>
-      </c>
-      <c r="I11" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J11" s="106">
-        <v>92</v>
-      </c>
-      <c r="K11" s="102" t="s">
-        <v>171</v>
-      </c>
-      <c r="L11" s="112">
-        <v>32</v>
-      </c>
-      <c r="M11" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="N11" s="113">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="102" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="103">
-        <v>12</v>
-      </c>
-      <c r="C12" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="104">
-        <v>97</v>
-      </c>
-      <c r="E12" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F12" s="106">
-        <v>100</v>
-      </c>
-      <c r="G12" s="102" t="s">
-        <v>169</v>
-      </c>
-      <c r="H12" s="112">
-        <v>69</v>
-      </c>
-      <c r="I12" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J12" s="113">
-        <v>57</v>
-      </c>
-      <c r="K12" s="102" t="s">
-        <v>176</v>
-      </c>
-      <c r="L12" s="112">
-        <v>71</v>
-      </c>
-      <c r="M12" s="105" t="s">
-        <v>173</v>
-      </c>
-      <c r="N12" s="113">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="102" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="103">
-        <v>103</v>
-      </c>
-      <c r="C13" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="104">
-        <v>100</v>
-      </c>
-      <c r="E13" s="105" t="s">
-        <v>163</v>
-      </c>
-      <c r="F13" s="106">
-        <v>100</v>
-      </c>
-      <c r="G13" s="102" t="s">
-        <v>166</v>
-      </c>
-      <c r="H13" s="104">
-        <v>92</v>
-      </c>
-      <c r="I13" s="105" t="s">
-        <v>166</v>
-      </c>
-      <c r="J13" s="113">
-        <v>64</v>
-      </c>
-      <c r="K13" s="102" t="s">
-        <v>173</v>
-      </c>
-      <c r="L13" s="112">
-        <v>76</v>
-      </c>
-      <c r="M13" s="105" t="s">
-        <v>171</v>
-      </c>
-      <c r="N13" s="113">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="103">
-        <v>86</v>
-      </c>
-      <c r="C14" s="102" t="s">
-        <v>163</v>
-      </c>
-      <c r="D14" s="104">
-        <v>94</v>
-      </c>
-      <c r="E14" s="105" t="s">
-        <v>165</v>
-      </c>
-      <c r="F14" s="113">
-        <v>52</v>
-      </c>
-      <c r="G14" s="102" t="s">
-        <v>168</v>
-      </c>
-      <c r="H14" s="112">
-        <v>71</v>
-      </c>
-      <c r="I14" s="105" t="s">
-        <v>168</v>
-      </c>
-      <c r="J14" s="113">
-        <v>85</v>
-      </c>
-      <c r="K14" s="102" t="s">
-        <v>171</v>
-      </c>
-      <c r="L14" s="104">
-        <v>99</v>
-      </c>
-      <c r="M14" s="105" t="s">
-        <v>171</v>
-      </c>
-      <c r="N14" s="113">
+      <c r="N14" s="119">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="63" t="s">
-        <v>196</v>
-      </c>
-      <c r="B15" s="107">
+        <v>188</v>
+      </c>
+      <c r="B15" s="92">
         <v>8</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>165</v>
-      </c>
-      <c r="D15" s="108">
+        <v>159</v>
+      </c>
+      <c r="D15" s="121">
         <v>99</v>
       </c>
-      <c r="E15" s="109" t="s">
+      <c r="E15" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="110" t="s">
+      <c r="F15" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="63" t="s">
-        <v>168</v>
-      </c>
-      <c r="H15" s="108">
+      <c r="G15" s="124" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" s="121">
         <v>100</v>
       </c>
-      <c r="I15" s="109" t="s">
+      <c r="I15" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="110" t="s">
+      <c r="J15" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="L15" s="114">
+      <c r="K15" s="124" t="s">
+        <v>171</v>
+      </c>
+      <c r="L15" s="121">
         <v>49</v>
       </c>
-      <c r="M15" s="109" t="s">
+      <c r="M15" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="110" t="s">
+      <c r="N15" s="123" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="111" t="s">
-        <v>197</v>
+      <c r="A16" s="93" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>